<commit_message>
Termianmos con defincion de procedures
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
   <si>
     <t>Method</t>
   </si>
@@ -235,6 +235,39 @@
   </si>
   <si>
     <t>Horarios disponibles de ese profesional para esa fecha y especialidad</t>
+  </si>
+  <si>
+    <t>topEspecialidadesMasCancelaciones()</t>
+  </si>
+  <si>
+    <t>especialidadDescripcion, cantidad</t>
+  </si>
+  <si>
+    <t>Cancelaciones tanto de afiliados como de profesionales</t>
+  </si>
+  <si>
+    <t>topProfesionalesMasConsultadosPorPlan()</t>
+  </si>
+  <si>
+    <t>planDescripcion, profesionalNombre, profesionalApellido, especialidadDescripcion, cantidad</t>
+  </si>
+  <si>
+    <t>Se calculan las consultas que un profesional tuvo para cada especialidad por separado</t>
+  </si>
+  <si>
+    <t>topProfesionalesMenosHoras(codigoPlan, codigoEspecialidad)</t>
+  </si>
+  <si>
+    <t>profesionalNombre, profesionalApellido, cantidad</t>
+  </si>
+  <si>
+    <t>topAfiliadosMasBonos()</t>
+  </si>
+  <si>
+    <t>nombreAfiliado, apellidoAfiliado, perteneceAGrupoFamiliar, cantidad</t>
+  </si>
+  <si>
+    <t>topEspecialidadesMasBonosUsados()</t>
   </si>
 </sst>
 </file>
@@ -631,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1074,40 +1107,64 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
+      <c r="A33" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="C34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
+      <c r="A35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="7"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="C36" s="3"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>

</xml_diff>

<commit_message>
Actualizo excel de procedures y creo el de triggers
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
   <si>
     <t>Method</t>
   </si>
@@ -84,9 +84,6 @@
     <t>login(username, password)</t>
   </si>
   <si>
-    <t>Recordar que luego de 3 intentos fallidos se debe deshabilitar al usuario</t>
-  </si>
-  <si>
     <t>obtenerRolesDeUsuario(idUsuario)</t>
   </si>
   <si>
@@ -96,21 +93,12 @@
     <t xml:space="preserve">Recordar poner estado como habilitado y asignar un numero de afiliado. Si se pasa una raíz, es cónyuge o hijo de un afiliado </t>
   </si>
   <si>
-    <t>modificarAfiliado(password, direccion, telefono, mail, sexo, estadoCivil, familiaresACargo, idPlanMedico)</t>
-  </si>
-  <si>
-    <t>Recordar que si se cambia el plan hay que agregar al anterior al historial de cambios de plan</t>
-  </si>
-  <si>
     <t>habilitarAfiliado(idAfiliado)</t>
   </si>
   <si>
     <t>eliminarAfiliado(idAfiliado)</t>
   </si>
   <si>
-    <t>Baja lógica (inhabilitar). Recordar dar de baja los turnos que tenía posteriores a la fecha de inhabilitación</t>
-  </si>
-  <si>
     <t>obtenerPlanesMedicos()</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
     <t>registrarLlegada(idAfiliado, numeroTurno, fecha)</t>
   </si>
   <si>
-    <t>Crear una consulta médica para ese turno y asignar un bono a esa consulta</t>
-  </si>
-  <si>
     <t>idAfiliado, nroAfiliado, codigoPlan, bonoConsulta</t>
   </si>
   <si>
@@ -268,6 +253,24 @@
   </si>
   <si>
     <t>topEspecialidadesMasBonosUsados()</t>
+  </si>
+  <si>
+    <t>Recordar que luego de 3 intentos fallidos se debe deshabilitar al usuario. Si el login es satisfactorio, limpiar intentos_login.</t>
+  </si>
+  <si>
+    <t>Baja lógica (inhabilitar). Recordar dar de baja los turnos que tenía posteriores a la fecha de inhabilitación para que otros los puedan usar.</t>
+  </si>
+  <si>
+    <t>Validar que el afiliado que los compra esté habilitado.</t>
+  </si>
+  <si>
+    <t>modificarAfiliado(password, direccion, telefono, mail, sexo, estadoCivil, familiaresACargo, idPlanMedico, motivo)</t>
+  </si>
+  <si>
+    <t>Recordar que si se cambia el plan hay que agregar al anterior al historial de cambios de plan. Motivo es opcional si se cambia el plan.</t>
+  </si>
+  <si>
+    <t>Crear una consulta médica para ese turno.</t>
   </si>
 </sst>
 </file>
@@ -664,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -701,7 +704,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -721,7 +724,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
@@ -796,7 +799,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -804,10 +807,10 @@
     </row>
     <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7"/>
       <c r="E9" s="2"/>
@@ -816,13 +819,13 @@
     </row>
     <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -830,13 +833,13 @@
     </row>
     <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>26</v>
+        <v>82</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -844,7 +847,7 @@
     </row>
     <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>14</v>
@@ -856,13 +859,13 @@
     </row>
     <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -870,10 +873,10 @@
     </row>
     <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3"/>
       <c r="E14" s="2"/>
@@ -882,10 +885,10 @@
     </row>
     <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C15" s="7"/>
       <c r="E15" s="2"/>
@@ -894,13 +897,13 @@
     </row>
     <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -908,13 +911,13 @@
     </row>
     <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -922,22 +925,24 @@
     </row>
     <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C19" s="7"/>
       <c r="E19" s="2"/>
@@ -946,10 +951,10 @@
     </row>
     <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C20" s="3"/>
       <c r="E20" s="2"/>
@@ -958,13 +963,13 @@
     </row>
     <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -972,13 +977,13 @@
     </row>
     <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -986,13 +991,13 @@
     </row>
     <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1000,13 +1005,13 @@
     </row>
     <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1014,13 +1019,13 @@
     </row>
     <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1028,7 +1033,7 @@
     </row>
     <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>14</v>
@@ -1040,10 +1045,10 @@
     </row>
     <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C27" s="7"/>
       <c r="E27" s="2"/>
@@ -1052,13 +1057,13 @@
     </row>
     <row r="28" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1066,13 +1071,13 @@
     </row>
     <row r="29" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1080,13 +1085,13 @@
     </row>
     <row r="30" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1094,13 +1099,13 @@
     </row>
     <row r="31" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1108,13 +1113,13 @@
     </row>
     <row r="32" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1122,13 +1127,13 @@
     </row>
     <row r="33" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1136,10 +1141,10 @@
     </row>
     <row r="34" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C34" s="3"/>
       <c r="E34" s="2"/>
@@ -1148,10 +1153,10 @@
     </row>
     <row r="35" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C35" s="7"/>
       <c r="E35" s="2"/>
@@ -1160,10 +1165,10 @@
     </row>
     <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C36" s="3"/>
       <c r="E36" s="2"/>

</xml_diff>

<commit_message>
Avance procedimientos y actualizacion de excel
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>Method</t>
   </si>
@@ -271,6 +266,18 @@
   </si>
   <si>
     <t>Crear una consulta médica para ese turno.</t>
+  </si>
+  <si>
+    <t>Pasar el id de usuario, Si cambia el plan debe recibir un motivo.</t>
+  </si>
+  <si>
+    <t>Se creo trigger de cambio de plan</t>
+  </si>
+  <si>
+    <t>Ver cuales son los posterirores a la fecha de baja</t>
+  </si>
+  <si>
+    <t>Ver como relacionar la agenda con el profesional</t>
   </si>
 </sst>
 </file>
@@ -352,15 +359,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,23 +676,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="84.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="7" max="7" width="41.875" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -700,10 +709,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -720,13 +729,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2">
@@ -735,15 +744,15 @@
       <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -751,51 +760,51 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="7"/>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -803,25 +812,25 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="5"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -829,77 +838,85 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="3"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="3"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="5"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -910,13 +927,13 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E17" s="2"/>
@@ -924,10 +941,10 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -938,22 +955,22 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="5"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C20" s="3"/>
@@ -962,13 +979,13 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>66</v>
       </c>
       <c r="E21" s="2"/>
@@ -976,10 +993,10 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -990,13 +1007,13 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="2"/>
@@ -1004,10 +1021,10 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1018,13 +1035,13 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>83</v>
       </c>
       <c r="E25" s="2"/>
@@ -1032,10 +1049,10 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="3"/>
@@ -1044,22 +1061,22 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="5"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -1070,13 +1087,13 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>56</v>
       </c>
       <c r="E29" s="2"/>
@@ -1084,10 +1101,10 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -1098,13 +1115,13 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>64</v>
       </c>
       <c r="E31" s="2"/>
@@ -1112,10 +1129,10 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -1126,13 +1143,13 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="5" t="s">
         <v>72</v>
       </c>
       <c r="E33" s="2"/>
@@ -1140,10 +1157,10 @@
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C34" s="3"/>
@@ -1152,22 +1169,22 @@
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="5"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C36" s="3"/>
@@ -1176,40 +1193,40 @@
       <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1218,7 +1235,7 @@
     <row r="42" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
+      <c r="C42" s="4"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1226,7 +1243,7 @@
     <row r="43" spans="1:7" ht="39.950000000000003" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
+      <c r="C43" s="4"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>

</xml_diff>

<commit_message>
Actualizo el excel con lo ultimo y agrego tres procedures
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
   <si>
     <t>Method</t>
   </si>
@@ -82,9 +87,6 @@
     <t>obtenerRolesDeUsuario(idUsuario)</t>
   </si>
   <si>
-    <t>crearAfiliado(username, password, nombre, apellido, dni, direccion, telefono, mail, fechaNac, sexo, estadoCivil, familiaresACargo, idPlanMedico, raizNumDeAfiliado)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recordar poner estado como habilitado y asignar un numero de afiliado. Si se pasa una raíz, es cónyuge o hijo de un afiliado </t>
   </si>
   <si>
@@ -112,9 +114,6 @@
     <t>codigoPlan, descripcion, bonoConsulta, bonoFarmacia</t>
   </si>
   <si>
-    <t>idProfesional, nombre, apellido, codigoEspecialidad, descripcionEspecialidad, idAgenda</t>
-  </si>
-  <si>
     <t>dia -&gt; String. horarios -&gt; entero de 0 a 25(semana), 7 a 16(sábados)</t>
   </si>
   <si>
@@ -133,12 +132,6 @@
     <t>codigoEspecialidad, descripcionEspecialidad</t>
   </si>
   <si>
-    <t>obtenerProfesionalPorEspecialidad(codigoEspecialidad)</t>
-  </si>
-  <si>
-    <t>idProfesional, nombre, apellido, idAgenda</t>
-  </si>
-  <si>
     <t>idHorario, horario,</t>
   </si>
   <si>
@@ -278,6 +271,30 @@
   </si>
   <si>
     <t>Ver como relacionar la agenda con el profesional</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>raiz</t>
+  </si>
+  <si>
+    <t>crearAfiliado(username, password, nombre, apellido, dni, direccion, telefono, mail, fechaNac, sexo, estadoCivil, familiaresACargo, idPlanMedico, numDeAfiliado)</t>
+  </si>
+  <si>
+    <t>obtenerRaizAfiliado()</t>
+  </si>
+  <si>
+    <t>idProfesional, nombre, apellido, codigoEspecialidad, descripcionEspecialidad</t>
+  </si>
+  <si>
+    <t>idProfesional, nombre, apellido</t>
+  </si>
+  <si>
+    <t>obtenerProfesionalesPorEspecialidad(codigoEspecialidad)</t>
   </si>
 </sst>
 </file>
@@ -674,21 +691,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" customWidth="1"/>
-    <col min="7" max="7" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="64.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="54.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.75" customWidth="1"/>
+    <col min="8" max="8" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -698,57 +716,66 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
+      <c r="D2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" s="2">
         <v>200</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1">
+    <row r="3" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2">
+      <c r="D3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" s="2">
         <v>400</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1">
+    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -758,11 +785,14 @@
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="D4" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -770,11 +800,14 @@
         <v>14</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -782,11 +815,14 @@
         <v>14</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -796,11 +832,14 @@
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="D7" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -808,445 +847,514 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="B16" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="2"/>
+      <c r="H16" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E18" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="E19" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="E20" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A21" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A21" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="2"/>
+      <c r="D23" s="3"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="5"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="E26" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A27" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="E27" s="2"/>
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="3"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A32" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="3"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A34" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="E34" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A34" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="5"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="E35" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A35" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="3"/>
-      <c r="E36" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C37" s="3"/>
-      <c r="E37" s="2"/>
+      <c r="D37" s="3"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
-      <c r="E38" s="2"/>
+      <c r="D38" s="3"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
-      <c r="E39" s="2"/>
+      <c r="D39" s="3"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
-      <c r="E40" s="2"/>
+      <c r="D40" s="3"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
-      <c r="E41" s="2"/>
+      <c r="D41" s="3"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="39.950000000000003" customHeight="1">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="E42" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" ht="39.950000000000003" customHeight="1">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="E43" s="2"/>
+      <c r="D43" s="4"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizo excel de procedures
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
   <si>
     <t>Method</t>
   </si>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1058,7 +1058,9 @@
         <v>90</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>

</xml_diff>

<commit_message>
Actualizo excel y subo obtner raiz afiliado y comprarBono
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
   <si>
     <t>Method</t>
   </si>
@@ -295,6 +290,9 @@
   </si>
   <si>
     <t>obtenerProfesionalesPorEspecialidad(codigoEspecialidad)</t>
+  </si>
+  <si>
+    <t>Se creo secuencia sq_numeroAfiliado</t>
   </si>
 </sst>
 </file>
@@ -693,17 +691,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="64.625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="54.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.75" customWidth="1"/>
-    <col min="8" max="8" width="41.875" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -879,10 +877,14 @@
         <v>86</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="3" t="s">
@@ -1030,7 +1032,9 @@
       <c r="C19" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>

</xml_diff>

<commit_message>
Agrego fecha_llegada a tabla Turno. Actualizo excel. Subo los procedures que hice.
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>Method</t>
   </si>
@@ -157,9 +162,6 @@
     <t>obtenerTurnosDeProfesional(idProfesional, fecha)</t>
   </si>
   <si>
-    <t>numeroTurno, fechaHorarioAtencion</t>
-  </si>
-  <si>
     <t>Todos los turnos del profesional para ese día</t>
   </si>
   <si>
@@ -253,9 +255,6 @@
     <t>Recordar que si se cambia el plan hay que agregar al anterior al historial de cambios de plan. Motivo es opcional si se cambia el plan.</t>
   </si>
   <si>
-    <t>Crear una consulta médica para ese turno.</t>
-  </si>
-  <si>
     <t>Pasar el id de usuario, Si cambia el plan debe recibir un motivo.</t>
   </si>
   <si>
@@ -293,6 +292,21 @@
   </si>
   <si>
     <t>Se creo secuencia sq_numeroAfiliado</t>
+  </si>
+  <si>
+    <t>obtenerCantidadDeBonosDisponiblesPorAfiliado(idAfiliado)</t>
+  </si>
+  <si>
+    <t>cantidadBonos</t>
+  </si>
+  <si>
+    <t>Actualizar consulta médica con resultados de la consulta.</t>
+  </si>
+  <si>
+    <t>Crear una consulta médica para ese turno y asociar un bono a esa consulta.</t>
+  </si>
+  <si>
+    <t>numeroTurno, fechaHorarioAtencion, nombreProfesional, apellidoProfesional, especialidad</t>
   </si>
 </sst>
 </file>
@@ -691,17 +705,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="56.375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="42.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="4" max="4" width="32.75" customWidth="1"/>
+    <col min="8" max="8" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -715,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -738,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -761,7 +775,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -784,7 +798,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -799,7 +813,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -814,7 +828,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -831,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -845,10 +859,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -863,7 +877,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -871,24 +885,24 @@
     </row>
     <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
@@ -897,7 +911,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -905,21 +919,21 @@
     </row>
     <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -931,12 +945,12 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -947,15 +961,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -967,7 +981,7 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -978,16 +992,16 @@
         <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -1016,7 +1030,7 @@
         <v>33</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1030,10 +1044,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1048,7 +1062,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1056,14 +1070,14 @@
     </row>
     <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1077,7 +1091,7 @@
         <v>37</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="2"/>
@@ -1092,7 +1106,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="3"/>
       <c r="F23" s="2"/>
@@ -1119,10 +1133,10 @@
         <v>46</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="3"/>
       <c r="F25" s="2"/>
@@ -1137,48 +1151,56 @@
         <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="C29" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3"/>
       <c r="F29" s="2"/>
@@ -1187,13 +1209,13 @@
     </row>
     <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="2"/>
@@ -1202,13 +1224,13 @@
     </row>
     <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="D31" s="3"/>
       <c r="F31" s="2"/>
@@ -1217,13 +1239,13 @@
     </row>
     <row r="32" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A32" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="2"/>
@@ -1232,13 +1254,13 @@
     </row>
     <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D33" s="3"/>
       <c r="F33" s="2"/>
@@ -1247,13 +1269,13 @@
     </row>
     <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="2"/>
@@ -1262,10 +1284,10 @@
     </row>
     <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1275,10 +1297,10 @@
     </row>
     <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A36" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1288,10 +1310,10 @@
     </row>
     <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1300,8 +1322,12 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
+      <c r="A38" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="2"/>

</xml_diff>

<commit_message>
Actualizo el Der y el excel
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -114,9 +114,6 @@
     <t>codigoPlan, descripcion, bonoConsulta, bonoFarmacia</t>
   </si>
   <si>
-    <t>dia -&gt; String. horarios -&gt; entero de 0 a 25(semana), 7 a 16(sábados)</t>
-  </si>
-  <si>
     <t>obtenerBonosPorNumeroAfiliado(nroAfiliado)</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t>numeroTurno, fechaHorarioAtencion, nombreProfesional, apellidoProfesional, especialidad</t>
+  </si>
+  <si>
+    <t>dia -&gt; int(1 - domingo). horarios -&gt; entero de 0 a 25(semana), 7 a 16(sábados)</t>
   </si>
 </sst>
 </file>
@@ -705,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -729,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -752,7 +752,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -775,7 +775,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -798,7 +798,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -813,7 +813,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -828,7 +828,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -845,7 +845,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -859,10 +859,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -885,24 +885,24 @@
     </row>
     <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
@@ -911,7 +911,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -919,21 +919,21 @@
     </row>
     <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -945,12 +945,12 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -961,15 +961,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -981,7 +981,7 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -992,27 +992,27 @@
         <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="D17" s="3"/>
       <c r="F17" s="2"/>
@@ -1021,16 +1021,16 @@
     </row>
     <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1038,16 +1038,16 @@
     </row>
     <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1055,14 +1055,14 @@
     </row>
     <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1070,14 +1070,14 @@
     </row>
     <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1085,13 +1085,13 @@
     </row>
     <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="2"/>
@@ -1100,13 +1100,13 @@
     </row>
     <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3"/>
       <c r="F23" s="2"/>
@@ -1115,13 +1115,13 @@
     </row>
     <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="2"/>
@@ -1130,13 +1130,13 @@
     </row>
     <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D25" s="3"/>
       <c r="F25" s="2"/>
@@ -1145,16 +1145,16 @@
     </row>
     <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1162,16 +1162,16 @@
     </row>
     <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1179,14 +1179,14 @@
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1194,13 +1194,13 @@
     </row>
     <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="C29" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="3"/>
       <c r="F29" s="2"/>
@@ -1209,13 +1209,13 @@
     </row>
     <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="2"/>
@@ -1224,28 +1224,28 @@
     </row>
     <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D31" s="3"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="32" spans="1:8" ht="45">
       <c r="A32" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="2"/>
@@ -1254,13 +1254,13 @@
     </row>
     <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D33" s="3"/>
       <c r="F33" s="2"/>
@@ -1269,13 +1269,13 @@
     </row>
     <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>67</v>
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="2"/>
@@ -1284,10 +1284,10 @@
     </row>
     <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1310,10 +1310,10 @@
     </row>
     <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>

</xml_diff>

<commit_message>
Actualizo der y excel
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="95">
   <si>
     <t>Method</t>
   </si>
@@ -138,9 +138,6 @@
     <t>registrarTurno(idAfiliado, idHorario)</t>
   </si>
   <si>
-    <t>registrarAgenda(idProfesional, fechaInicio, fechaFin, Table[dia, horarioInicio, horarioFin, codigoEspecialidad])</t>
-  </si>
-  <si>
     <t>registrarLlegada(idAfiliado, numeroTurno, fecha)</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Todos los turnos del profesional para ese día</t>
   </si>
   <si>
-    <t>No se puede sacar turno si no tiene bonos disponibles</t>
-  </si>
-  <si>
     <t>numeroTurno, fechaHorarioAtencion, numeroAfiliado, nombreAfiliado, apellidoAfiliado</t>
   </si>
   <si>
@@ -306,7 +300,10 @@
     <t>numeroTurno, fechaHorarioAtencion, nombreProfesional, apellidoProfesional, especialidad</t>
   </si>
   <si>
-    <t>dia -&gt; int(1 - domingo). horarios -&gt; entero de 0 a 25(semana), 7 a 16(sábados)</t>
+    <t>registrarAgenda(idProfesional, mesInicio, mesFin, Table[dia, horarioInicio, horarioFin, codigoEspecialidad])</t>
+  </si>
+  <si>
+    <t>dia -&gt; int(1 - domingo). horarios -&gt; datetime. Mes -&gt; 0 - Enero</t>
   </si>
 </sst>
 </file>
@@ -705,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +726,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -752,7 +749,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -775,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -798,7 +795,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -813,7 +810,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -828,7 +825,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -845,7 +842,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -859,10 +856,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -877,7 +874,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -885,24 +882,24 @@
     </row>
     <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
@@ -911,7 +908,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -919,21 +916,21 @@
     </row>
     <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -945,12 +942,12 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -961,15 +958,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -981,7 +978,7 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -992,27 +989,27 @@
         <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="3"/>
       <c r="F17" s="2"/>
@@ -1024,13 +1021,13 @@
         <v>31</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1044,10 +1041,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1062,7 +1059,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1070,14 +1067,14 @@
     </row>
     <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1091,7 +1088,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="2"/>
@@ -1105,9 +1102,7 @@
       <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1115,13 +1110,13 @@
     </row>
     <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D24" s="5"/>
       <c r="F24" s="2"/>
@@ -1130,13 +1125,13 @@
     </row>
     <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D25" s="3"/>
       <c r="F25" s="2"/>
@@ -1145,16 +1140,16 @@
     </row>
     <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1162,16 +1157,16 @@
     </row>
     <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1179,14 +1174,14 @@
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1194,13 +1189,13 @@
     </row>
     <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D29" s="3"/>
       <c r="F29" s="2"/>
@@ -1209,13 +1204,13 @@
     </row>
     <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="2"/>
@@ -1224,13 +1219,13 @@
     </row>
     <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D31" s="3"/>
       <c r="F31" s="2"/>
@@ -1239,13 +1234,13 @@
     </row>
     <row r="32" spans="1:8" ht="45">
       <c r="A32" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="2"/>
@@ -1254,13 +1249,13 @@
     </row>
     <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="D33" s="3"/>
       <c r="F33" s="2"/>
@@ -1269,13 +1264,13 @@
     </row>
     <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="2"/>
@@ -1284,10 +1279,10 @@
     </row>
     <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1297,10 +1292,10 @@
     </row>
     <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1310,10 +1305,10 @@
     </row>
     <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1323,10 +1318,10 @@
     </row>
     <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>

</xml_diff>

<commit_message>
Actualizo excel. Subo procedures
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
   <si>
     <t>Method</t>
   </si>
@@ -144,9 +144,6 @@
     <t>idAfiliado, nroAfiliado, codigoPlan, bonoConsulta</t>
   </si>
   <si>
-    <t>obtenerProfesionalesDelDiaPor(nombre, apellido, especialidad, fecha)</t>
-  </si>
-  <si>
     <t>Profesionales que atiendan ese dia y cumplan con los filtros</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Todos los turnos del profesional para ese día</t>
   </si>
   <si>
-    <t>numeroTurno, fechaHorarioAtencion, numeroAfiliado, nombreAfiliado, apellidoAfiliado</t>
-  </si>
-  <si>
     <t>registrarAtencionMedica(numeroTurno, fecha, sintomas, diagnostico)</t>
   </si>
   <si>
@@ -304,18 +298,31 @@
   </si>
   <si>
     <t>dia -&gt; int(1 - domingo). horarios -&gt; datetime. Mes -&gt; 0 - Enero</t>
+  </si>
+  <si>
+    <t>obtenerProfesionalesDelDiaPor(nombre, apellido, codEspecialidad, fecha)</t>
+  </si>
+  <si>
+    <t>numeroTurno, idAfiliado, numeroAfiliado, nombreAfiliado, apellidoAfiliado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -327,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +350,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -374,9 +387,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -391,11 +404,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -726,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -748,8 +770,8 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>80</v>
+      <c r="D2" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -771,8 +793,8 @@
       <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>80</v>
+      <c r="D3" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -794,8 +816,8 @@
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>80</v>
+      <c r="D4" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -809,8 +831,8 @@
         <v>14</v>
       </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>80</v>
+      <c r="D5" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -824,8 +846,8 @@
         <v>14</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>80</v>
+      <c r="D6" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -841,8 +863,8 @@
       <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>80</v>
+      <c r="D7" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -856,10 +878,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -873,8 +895,8 @@
         <v>29</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>80</v>
+      <c r="D9" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -882,24 +904,24 @@
     </row>
     <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
-        <v>80</v>
+      <c r="D10" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
@@ -907,8 +929,8 @@
       <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>80</v>
+      <c r="D11" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -916,21 +938,21 @@
     </row>
     <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>80</v>
+        <v>72</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -941,13 +963,13 @@
         <v>14</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>80</v>
+      <c r="D13" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -958,15 +980,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>80</v>
+        <v>69</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -977,8 +999,8 @@
         <v>30</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>80</v>
+      <c r="D15" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -989,29 +1011,31 @@
         <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>80</v>
+      <c r="D16" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>92</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1026,8 +1050,8 @@
       <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>80</v>
+      <c r="D18" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1041,10 +1065,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1058,8 +1082,8 @@
         <v>35</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>80</v>
+      <c r="D20" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -1067,14 +1091,14 @@
     </row>
     <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>80</v>
+      <c r="D21" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1088,7 +1112,7 @@
         <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22" s="2"/>
@@ -1103,37 +1127,43 @@
         <v>14</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1146,10 +1176,10 @@
         <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>80</v>
+        <v>89</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1157,16 +1187,16 @@
     </row>
     <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1174,14 +1204,14 @@
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
-        <v>80</v>
+      <c r="D28" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1189,13 +1219,13 @@
     </row>
     <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3"/>
       <c r="F29" s="2"/>
@@ -1204,13 +1234,13 @@
     </row>
     <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D30" s="5"/>
       <c r="F30" s="2"/>
@@ -1219,13 +1249,13 @@
     </row>
     <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D31" s="3"/>
       <c r="F31" s="2"/>
@@ -1234,13 +1264,13 @@
     </row>
     <row r="32" spans="1:8" ht="45">
       <c r="A32" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D32" s="5"/>
       <c r="F32" s="2"/>
@@ -1249,13 +1279,13 @@
     </row>
     <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D33" s="3"/>
       <c r="F33" s="2"/>
@@ -1264,13 +1294,13 @@
     </row>
     <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D34" s="5"/>
       <c r="F34" s="2"/>
@@ -1279,10 +1309,10 @@
     </row>
     <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1292,10 +1322,10 @@
     </row>
     <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1305,10 +1335,10 @@
     </row>
     <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1317,14 +1347,16 @@
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
-      <c r="A38" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
+      <c r="A38" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -1385,6 +1417,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizo excel y ProcedimientoVictor con topEspecialidadesMasCancelaciones
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="97">
   <si>
     <t>Method</t>
   </si>
@@ -304,6 +299,12 @@
   </si>
   <si>
     <t>numeroTurno, idAfiliado, numeroAfiliado, nombreAfiliado, apellidoAfiliado</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>Ver a que se refiere por Afiliado y Profesional</t>
   </si>
 </sst>
 </file>
@@ -724,17 +725,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56.375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="42.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.25" customWidth="1"/>
-    <col min="4" max="4" width="32.75" customWidth="1"/>
-    <col min="8" max="8" width="41.875" customWidth="1"/>
+    <col min="1" max="1" width="56.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="8" max="8" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1">
@@ -1262,7 +1261,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:8" ht="60">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
@@ -1287,10 +1286,14 @@
       <c r="C33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="H33" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
       <c r="A34" s="5" t="s">

</xml_diff>

<commit_message>
agrego procedure obtenerHorariosDisponiblesParaFecha y actualizo excel
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\Matias\UTN\Gestión de Datos\TP\Clinica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\FACU TPS\TP CLINICA FRBA 1.0 - 2C 2016\Clinica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="96">
   <si>
     <t>Method</t>
   </si>
@@ -304,12 +304,15 @@
   </si>
   <si>
     <t>numeroTurno, idAfiliado, numeroAfiliado, nombreAfiliado, apellidoAfiliado</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -724,20 +727,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="56.375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="42.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.25" customWidth="1"/>
-    <col min="4" max="4" width="32.75" customWidth="1"/>
-    <col min="8" max="8" width="41.875" customWidth="1"/>
+    <col min="1" max="1" width="56.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.21875" customWidth="1"/>
+    <col min="4" max="4" width="32.77734375" customWidth="1"/>
+    <col min="8" max="8" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:8" ht="39.9" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -760,7 +763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="1:8" ht="39.9" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -783,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="3" spans="1:8" ht="39.9" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -806,7 +809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="4" spans="1:8" ht="39.9" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -823,7 +826,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="5" spans="1:8" ht="39.9" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -838,7 +841,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="6" spans="1:8" ht="39.9" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -853,7 +856,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="7" spans="1:8" ht="39.9" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -870,7 +873,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:8" ht="39.9" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -887,7 +890,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="9" spans="1:8" ht="39.9" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -902,7 +905,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="10" spans="1:8" ht="39.9" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>81</v>
       </c>
@@ -919,7 +922,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="11" spans="1:8" ht="39.9" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>80</v>
       </c>
@@ -936,7 +939,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="12" spans="1:8" ht="39.9" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>71</v>
       </c>
@@ -955,7 +958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="13" spans="1:8" ht="39.9" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -972,7 +975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="14" spans="1:8" ht="39.9" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
@@ -991,7 +994,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="15" spans="1:8" ht="39.9" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -1006,7 +1009,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="16" spans="1:8" ht="39.9" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="17" spans="1:8" ht="39.9" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>91</v>
       </c>
@@ -1040,7 +1043,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="18" spans="1:8" ht="39.9" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -1057,7 +1060,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="19" spans="1:8" ht="39.9" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1074,7 +1077,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="20" spans="1:8" ht="39.9" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1089,7 +1092,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="21" spans="1:8" ht="39.9" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>84</v>
       </c>
@@ -1104,7 +1107,7 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="22" spans="1:8" ht="39.9" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
@@ -1114,12 +1117,14 @@
       <c r="C22" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="23" spans="1:8" ht="39.9" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
@@ -1134,7 +1139,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="24" spans="1:8" ht="39.9" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>93</v>
       </c>
@@ -1151,7 +1156,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="25" spans="1:8" ht="39.9" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>43</v>
       </c>
@@ -1168,7 +1173,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="26" spans="1:8" ht="39.9" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -1185,7 +1190,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="27" spans="1:8" ht="39.9" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1202,7 +1207,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="28" spans="1:8" ht="39.9" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
@@ -1217,7 +1222,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="29" spans="1:8" ht="39.9" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>48</v>
       </c>
@@ -1232,7 +1237,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="30" spans="1:8" ht="39.9" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
@@ -1247,7 +1252,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="31" spans="1:8" ht="39.9" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>51</v>
       </c>
@@ -1262,7 +1267,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:8" ht="43.2">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
@@ -1277,7 +1282,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="33" spans="1:8" ht="39.9" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>57</v>
       </c>
@@ -1292,7 +1297,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="34" spans="1:8" ht="39.9" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>60</v>
       </c>
@@ -1307,7 +1312,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="35" spans="1:8" ht="39.9" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>63</v>
       </c>
@@ -1320,7 +1325,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="36" spans="1:8" ht="39.9" customHeight="1">
       <c r="A36" s="5" t="s">
         <v>65</v>
       </c>
@@ -1333,7 +1338,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="37" spans="1:8" ht="39.9" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>67</v>
       </c>
@@ -1346,7 +1351,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="38" spans="1:8" ht="39.9" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>86</v>
       </c>
@@ -1361,7 +1366,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="39" spans="1:8" ht="39.9" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1370,7 +1375,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="40" spans="1:8" ht="39.9" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1379,7 +1384,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="41" spans="1:8" ht="39.9" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1388,7 +1393,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="42" spans="1:8" ht="39.9" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1397,7 +1402,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="43" spans="1:8" ht="39.9" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1406,7 +1411,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="44" spans="1:8" ht="39.9" customHeight="1">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>

</xml_diff>

<commit_message>
Agrego todos los procedures qe faltaban, solo falta 1 ver excel
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\FACU TPS\TP CLINICA FRBA 1.0 - 2C 2016\Clinica\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
   <si>
     <t>Method</t>
   </si>
@@ -169,15 +174,9 @@
     <t>cancelarTurnoPorAfiliado(idAfiliado, numeroTurno, tipoCancelacion, motivoCancelacion)</t>
   </si>
   <si>
-    <t>cancelarDiaPorProfesional(idProfesional, fecha)</t>
-  </si>
-  <si>
     <t>Se cancela el día entero</t>
   </si>
   <si>
-    <t>cancelarTurnosPorProfesional(idProfesional, fechaInicial, fechaFinal)</t>
-  </si>
-  <si>
     <t>Se cancelan todos los turnos que esten dentro de ese rango de fechas. Aplica siempre para un mismo día, no pueden tener distinta fecha</t>
   </si>
   <si>
@@ -302,12 +301,21 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>cancelarDiaPorProfesional(idProfesional, fecha,tipoCancelacion,motivo)</t>
+  </si>
+  <si>
+    <t>cancelarTurnosPorProfesional(idProfesional, fechaInicial, fechaFinal,tipoCancelacion,motivo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -722,20 +730,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="56.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="8" max="8" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:8" ht="39.9" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -746,7 +754,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -758,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="2" spans="1:8" ht="39.9" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -769,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F2" s="2">
         <v>200</v>
@@ -781,7 +789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="3" spans="1:8" ht="39.9" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -792,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2">
         <v>400</v>
@@ -804,7 +812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="4" spans="1:8" ht="39.9" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -815,13 +823,13 @@
         <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="5" spans="1:8" ht="39.9" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -830,13 +838,13 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="6" spans="1:8" ht="39.9" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -845,13 +853,13 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="7" spans="1:8" ht="39.9" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -862,13 +870,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:8" ht="39.9" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -876,16 +884,16 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="9" spans="1:8" ht="39.9" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -894,32 +902,32 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="10" spans="1:8" ht="39.9" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="39.9" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
@@ -928,32 +936,32 @@
         <v>22</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="12" spans="1:8" ht="39.9" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="39.9" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -962,15 +970,15 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="39.9" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
@@ -978,18 +986,18 @@
         <v>14</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="39.9" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>25</v>
       </c>
@@ -998,47 +1006,47 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="16" spans="1:8" ht="39.9" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="39.9" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="18" spans="1:8" ht="39.9" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -1049,13 +1057,13 @@
         <v>32</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="19" spans="1:8" ht="39.9" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
@@ -1063,16 +1071,16 @@
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="20" spans="1:8" ht="39.9" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
@@ -1081,28 +1089,28 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="21" spans="1:8" ht="39.9" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="22" spans="1:8" ht="39.9" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
@@ -1110,16 +1118,16 @@
         <v>36</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="23" spans="1:8" ht="39.9" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
@@ -1128,15 +1136,15 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="24" spans="1:8" ht="39.9" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>42</v>
@@ -1145,30 +1153,30 @@
         <v>41</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="25" spans="1:8" ht="39.9" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="26" spans="1:8" ht="39.9" customHeight="1">
       <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
@@ -1176,16 +1184,16 @@
         <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="27" spans="1:8" ht="39.9" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1193,31 +1201,31 @@
         <v>14</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="28" spans="1:8" ht="39.9" customHeight="1">
       <c r="A28" s="5" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="29" spans="1:8" ht="39.9" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>48</v>
       </c>
@@ -1225,14 +1233,16 @@
         <v>49</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="30" spans="1:8" ht="39.9" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>50</v>
       </c>
@@ -1242,96 +1252,102 @@
       <c r="C30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="31" spans="1:8" ht="39.9" customHeight="1">
       <c r="A31" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="60">
+    <row r="32" spans="1:8" ht="43.2">
       <c r="A32" s="5" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="33" spans="1:8" ht="39.9" customHeight="1">
       <c r="A33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="D33" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="34" spans="1:8" ht="39.9" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="D34" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="35" spans="1:8" ht="39.9" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="36" spans="1:8" ht="39.9" customHeight="1">
       <c r="A36" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1339,35 +1355,37 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="37" spans="1:8" ht="39.9" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
+      <c r="D37" s="8" t="s">
+        <v>76</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="38" spans="1:8" ht="39.9" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="39" spans="1:8" ht="39.9" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1376,7 +1394,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="40" spans="1:8" ht="39.9" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1385,7 +1403,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="41" spans="1:8" ht="39.9" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1394,7 +1412,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="42" spans="1:8" ht="39.9" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1403,7 +1421,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="43" spans="1:8" ht="39.9" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1412,7 +1430,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="44" spans="1:8" ht="39.9" customHeight="1">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>

</xml_diff>

<commit_message>
Termino utlimo procedure topAfiliadoConMasBonosComprados
</commit_message>
<xml_diff>
--- a/Procedures.xlsx
+++ b/Procedures.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="97">
   <si>
     <t>Method</t>
   </si>
@@ -730,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1350,7 +1350,9 @@
         <v>64</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="8" t="s">
+        <v>94</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>

</xml_diff>